<commit_message>
updating du dup python scripts
</commit_message>
<xml_diff>
--- a/DOM_Banner/output/test/H H Sherry Chow_2023.xlsx
+++ b/DOM_Banner/output/test/H H Sherry Chow_2023.xlsx
@@ -1066,7 +1066,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4361815215</t>
+          <t>https://openalex.org/W4361815056</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481174</t>
+          <t>https://doi.org/10.1158/1078-0432.22481174.v1</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1131,7 +1131,7 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481174</t>
+          <t>https://doi.org/10.1158/1078-0432.22481174.v1</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -1153,12 +1153,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4361815298</t>
+          <t>https://openalex.org/W4361815064</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Figure S2 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
+          <t>Table S2 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1178,7 +1178,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481183</t>
+          <t>https://doi.org/10.1158/1078-0432.22481171.v1</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481183</t>
+          <t>https://doi.org/10.1158/1078-0432.22481171.v1</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -1240,12 +1240,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4361815443</t>
+          <t>https://openalex.org/W4361815215</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Figure S2 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
+          <t>Table S1 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1265,7 +1265,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481183.v1</t>
+          <t>https://doi.org/10.1158/1078-0432.22481174</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1305,7 +1305,7 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481183.v1</t>
+          <t>https://doi.org/10.1158/1078-0432.22481174</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -1327,12 +1327,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4361815506</t>
+          <t>https://openalex.org/W4361815217</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Figure S3 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
+          <t>Figure S1 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1352,7 +1352,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481180</t>
+          <t>https://doi.org/10.1158/1078-0432.22481186</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1392,7 +1392,7 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481180</t>
+          <t>https://doi.org/10.1158/1078-0432.22481186</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
@@ -1414,12 +1414,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4361890113</t>
+          <t>https://openalex.org/W4361815298</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Table S3 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
+          <t>Figure S2 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481168</t>
+          <t>https://doi.org/10.1158/1078-0432.22481183</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1479,7 +1479,7 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481168</t>
+          <t>https://doi.org/10.1158/1078-0432.22481183</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
@@ -1491,32 +1491,32 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Srinivasan Vedantham, Hsin Wu Tseng, Zhiyang Fu, H.‐H. Sherry Chow</t>
+          <t>Patricia A. Thompson, Chuan Huang, Jie Yang, Betsy C. Wertheim, Denise J. Roe, Xiaoyue Zhang, Jie Ding, Pavani Chalasani, Christina Preece, Jessica Martínez, H.‐H. Sherry Chow, Alison Stopeck</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Department of Biomedical Engineering, University of Arizona, Tucson, AZ 85724, USA; Department of Medical Imaging, University of Arizona, Tucson, AZ 85724, USA; Department of Medical Imaging, University of Arizona, Tucson, AZ 85724, USA; Department of Medical Imaging, University of Arizona, Tucson, AZ 85724, USA; Department of Medicine, University of Arizona, Tucson, AZ 85724, USA</t>
+          <t xml:space="preserve">; ; ; ; ; ; ; ; ; ; ; </t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4388226308</t>
+          <t>https://openalex.org/W4361815443</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Dedicated Cone-Beam Breast CT: Reproducibility of Volumetric Glandular Fraction with Advanced Image Reconstruction Methods</t>
+          <t>Figure S2 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>2023-03-31</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Tomography</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://doi.org/10.3390/tomography9060160</t>
+          <t>https://doi.org/10.1158/1078-0432.22481183.v1</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1536,12 +1536,12 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>publishedVersion</t>
+          <t>submittedVersion</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>gold</t>
+          <t>green</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1561,12 +1561,12 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>https://pubmed.ncbi.nlm.nih.gov/37987346</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>https://doi.org/10.3390/tomography9060160</t>
+          <t>https://doi.org/10.1158/1078-0432.22481183.v1</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
@@ -1588,12 +1588,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4361815056</t>
+          <t>https://openalex.org/W4361815506</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Table S1 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
+          <t>Figure S3 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481174.v1</t>
+          <t>https://doi.org/10.1158/1078-0432.22481180</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1653,7 +1653,7 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481174.v1</t>
+          <t>https://doi.org/10.1158/1078-0432.22481180</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4361815064</t>
+          <t>https://openalex.org/W4361815613</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1700,7 +1700,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481171.v1</t>
+          <t>https://doi.org/10.1158/1078-0432.22481171</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481171.v1</t>
+          <t>https://doi.org/10.1158/1078-0432.22481171</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
@@ -1762,12 +1762,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4361815217</t>
+          <t>https://openalex.org/W4361815737</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Figure S1 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
+          <t>Data from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1787,12 +1787,12 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481186</t>
+          <t>https://doi.org/10.1158/1078-0432.c.6530630.v1</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>cc-by</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1827,7 +1827,7 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481186</t>
+          <t>https://doi.org/10.1158/1078-0432.c.6530630.v1</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
@@ -1849,12 +1849,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4361815613</t>
+          <t>https://openalex.org/W4361890113</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Table S2 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
+          <t>Table S3 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481171</t>
+          <t>https://doi.org/10.1158/1078-0432.22481168</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1914,7 +1914,7 @@
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481171</t>
+          <t>https://doi.org/10.1158/1078-0432.22481168</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
@@ -1936,12 +1936,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4361815737</t>
+          <t>https://openalex.org/W4361890117</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Data from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
+          <t>Table S4 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1961,12 +1961,12 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.c.6530630.v1</t>
+          <t>https://doi.org/10.1158/1078-0432.22481165</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>cc-by</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -2001,7 +2001,7 @@
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.c.6530630.v1</t>
+          <t>https://doi.org/10.1158/1078-0432.22481165</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4361890117</t>
+          <t>https://openalex.org/W4361939742</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2048,7 +2048,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481165</t>
+          <t>https://doi.org/10.1158/1078-0432.22481165.v1</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2088,7 +2088,7 @@
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481165</t>
+          <t>https://doi.org/10.1158/1078-0432.22481165.v1</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
@@ -2110,12 +2110,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4361939742</t>
+          <t>https://openalex.org/W4361939778</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Table S4 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
+          <t>Table S3 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2135,7 +2135,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481165.v1</t>
+          <t>https://doi.org/10.1158/1078-0432.22481168.v1</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2175,7 +2175,7 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481165.v1</t>
+          <t>https://doi.org/10.1158/1078-0432.22481168.v1</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
@@ -2187,32 +2187,32 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Patricia A. Thompson, Chuan Huang, Jie Yang, Betsy C. Wertheim, Denise J. Roe, Xiaoyue Zhang, Jie Ding, Pavani Chalasani, Christina Preece, Jessica Martínez, H.‐H. Sherry Chow, Alison Stopeck</t>
+          <t>Srinivasan Vedantham, Hsin Wu Tseng, Zhiyang Fu, H.‐H. Sherry Chow</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">; ; ; ; ; ; ; ; ; ; ; </t>
+          <t>Department of Biomedical Engineering, University of Arizona, Tucson, AZ 85724, USA; Department of Medical Imaging, University of Arizona, Tucson, AZ 85724, USA; Department of Medical Imaging, University of Arizona, Tucson, AZ 85724, USA; Department of Medical Imaging, University of Arizona, Tucson, AZ 85724, USA; Department of Medicine, University of Arizona, Tucson, AZ 85724, USA</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4361939778</t>
+          <t>https://openalex.org/W4388226308</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Table S3 from Sulindac, a Nonselective NSAID, Reduces Breast Density in Postmenopausal Women with Breast Cancer Treated with Aromatase Inhibitors</t>
+          <t>Dedicated Cone-Beam Breast CT: Reproducibility of Volumetric Glandular Fraction with Advanced Image Reconstruction Methods</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-11-02</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Tomography</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -2222,7 +2222,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481168.v1</t>
+          <t>https://doi.org/10.3390/tomography9060160</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -2232,12 +2232,12 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>submittedVersion</t>
+          <t>publishedVersion</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>green</t>
+          <t>gold</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2257,12 +2257,12 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>https://pubmed.ncbi.nlm.nih.gov/37987346</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1158/1078-0432.22481168.v1</t>
+          <t>https://doi.org/10.3390/tomography9060160</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">

</xml_diff>